<commit_message>
first day after feeling sick af
</commit_message>
<xml_diff>
--- a/Docs/timesheet.xlsx
+++ b/Docs/timesheet.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26924"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Libraries\Documents\School\Y2\Personal Portfolio\pp2\UnrealEngineBasics\Docs\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Alex\Documents\School\Y2\Personal Portfolio\pp2\UnrealEngineBasics\Docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BC8CFD84-040D-46AE-9FF4-8FA2D163AD16}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E36C2B11-E3C0-44C2-BF16-4EA8A2F73B1A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -112,12 +112,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="2" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
@@ -399,10 +397,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:H23"/>
+  <dimension ref="A1:L36"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B18" sqref="B18"/>
+      <selection activeCell="C15" sqref="C15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -416,385 +414,742 @@
     <col min="7" max="7" width="15.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A1" s="4" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="4" t="s">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A1" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="4" t="s">
+      <c r="C1" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="4" t="s">
+      <c r="D1" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="4" t="s">
+      <c r="E1" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="4" t="s">
+      <c r="F1" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="G1" s="4" t="s">
+      <c r="G1" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="H1" s="4" t="s">
+      <c r="H1" s="3" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A2" s="4" t="s">
+      <c r="I1" s="1"/>
+      <c r="J1" s="1"/>
+      <c r="K1" s="1"/>
+      <c r="L1" s="1"/>
+    </row>
+    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A2" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="B2" s="5">
+      <c r="B2" s="3">
         <v>10</v>
       </c>
-      <c r="C2" s="5">
+      <c r="C2" s="3">
         <v>30</v>
       </c>
-      <c r="D2" s="5">
+      <c r="D2" s="3">
         <v>10</v>
       </c>
-      <c r="E2" s="5">
+      <c r="E2" s="3">
         <v>30</v>
       </c>
-      <c r="F2" s="5">
+      <c r="F2" s="3">
         <f t="shared" ref="F2:F3" si="0">SUM(B2:E2)</f>
         <v>80</v>
       </c>
-    </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A3" s="4" t="s">
+      <c r="G2" s="1"/>
+      <c r="H2" s="1"/>
+      <c r="I2" s="1"/>
+      <c r="J2" s="1"/>
+      <c r="K2" s="1"/>
+      <c r="L2" s="1"/>
+    </row>
+    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A3" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="B3" s="2">
+      <c r="B3" s="1">
         <f>SUM(B5:B23)</f>
-        <v>0.48333333333333328</v>
-      </c>
-      <c r="C3" s="2">
+        <v>0.56666666666666665</v>
+      </c>
+      <c r="C3" s="1">
         <f>SUM(C5:C32)</f>
-        <v>10.216666666666667</v>
-      </c>
-      <c r="D3" s="2">
+        <v>11.45</v>
+      </c>
+      <c r="D3" s="1">
         <f>SUM(D5:D32)</f>
         <v>3.55</v>
       </c>
-      <c r="E3" s="2">
+      <c r="E3" s="1">
         <f>SUM(E5:E32)</f>
         <v>0.36666666666666664</v>
       </c>
-      <c r="F3" s="2">
+      <c r="F3" s="1">
         <f t="shared" si="0"/>
-        <v>14.616666666666667</v>
-      </c>
-      <c r="G3" s="2">
+        <v>15.933333333333334</v>
+      </c>
+      <c r="G3" s="1">
         <v>2</v>
       </c>
-      <c r="H3" s="2">
+      <c r="H3" s="1">
         <f>F3+G3</f>
-        <v>16.616666666666667</v>
-      </c>
-    </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A4" s="4" t="s">
+        <v>17.933333333333334</v>
+      </c>
+      <c r="I3" s="1"/>
+      <c r="J3" s="1"/>
+      <c r="K3" s="1"/>
+      <c r="L3" s="1"/>
+    </row>
+    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A4" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="B4" s="3">
+      <c r="B4" s="2">
         <f>(B3/B2)</f>
-        <v>4.8333333333333325E-2</v>
-      </c>
-      <c r="C4" s="3">
+        <v>5.6666666666666664E-2</v>
+      </c>
+      <c r="C4" s="2">
         <f t="shared" ref="C4:E4" si="1">(C3/C2)</f>
-        <v>0.34055555555555556</v>
-      </c>
-      <c r="D4" s="3">
+        <v>0.38166666666666665</v>
+      </c>
+      <c r="D4" s="2">
         <f t="shared" si="1"/>
         <v>0.35499999999999998</v>
       </c>
-      <c r="E4" s="3">
+      <c r="E4" s="2">
         <f t="shared" si="1"/>
         <v>1.2222222222222221E-2</v>
       </c>
-      <c r="F4" s="3">
+      <c r="F4" s="2">
         <f>(F3/F2)</f>
-        <v>0.18270833333333333</v>
-      </c>
-    </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+        <v>0.19916666666666666</v>
+      </c>
+      <c r="G4" s="1"/>
+      <c r="H4" s="1"/>
+      <c r="I4" s="1"/>
+      <c r="J4" s="1"/>
+      <c r="K4" s="1"/>
+      <c r="L4" s="1"/>
+    </row>
+    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A5" s="1">
         <v>45209</v>
       </c>
-      <c r="B5" s="2">
-        <f>0</f>
-        <v>0</v>
-      </c>
-      <c r="C5" s="2">
+      <c r="B5" s="1">
+        <f>0</f>
+        <v>0</v>
+      </c>
+      <c r="C5" s="1">
         <v>1</v>
       </c>
-      <c r="D5" s="2">
-        <f>0</f>
-        <v>0</v>
-      </c>
-      <c r="E5" s="2">
-        <f>0</f>
-        <v>0</v>
-      </c>
-      <c r="F5" s="2">
-        <f t="shared" ref="F5:F13" si="2">SUM(B5:E5)</f>
+      <c r="D5" s="1">
+        <f>0</f>
+        <v>0</v>
+      </c>
+      <c r="E5" s="1">
+        <f>0</f>
+        <v>0</v>
+      </c>
+      <c r="F5" s="1">
+        <f t="shared" ref="F5:F14" si="2">SUM(B5:E5)</f>
         <v>1</v>
       </c>
-    </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="G5" s="1"/>
+      <c r="H5" s="1"/>
+      <c r="I5" s="1"/>
+      <c r="J5" s="1"/>
+      <c r="K5" s="1"/>
+      <c r="L5" s="1"/>
+    </row>
+    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A6" s="1">
         <v>45211</v>
       </c>
-      <c r="B6" s="2">
-        <f>0</f>
-        <v>0</v>
-      </c>
-      <c r="C6" s="2">
+      <c r="B6" s="1">
+        <f>0</f>
+        <v>0</v>
+      </c>
+      <c r="C6" s="1">
         <v>0.5</v>
       </c>
-      <c r="D6" s="2">
+      <c r="D6" s="1">
         <v>0.5</v>
       </c>
-      <c r="E6" s="2">
-        <f>0</f>
-        <v>0</v>
-      </c>
-      <c r="F6" s="2">
+      <c r="E6" s="1">
+        <f>0</f>
+        <v>0</v>
+      </c>
+      <c r="F6" s="1">
         <f t="shared" si="2"/>
         <v>1</v>
       </c>
-    </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="G6" s="1"/>
+      <c r="H6" s="1"/>
+      <c r="I6" s="1"/>
+      <c r="J6" s="1"/>
+      <c r="K6" s="1"/>
+      <c r="L6" s="1"/>
+    </row>
+    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A7" s="1">
         <v>45217</v>
       </c>
-      <c r="B7" s="2">
-        <f>0</f>
-        <v>0</v>
-      </c>
-      <c r="C7" s="2">
+      <c r="B7" s="1">
+        <f>0</f>
+        <v>0</v>
+      </c>
+      <c r="C7" s="1">
         <v>1.5</v>
       </c>
-      <c r="D7" s="2">
+      <c r="D7" s="1">
         <v>1.25</v>
       </c>
-      <c r="E7" s="2">
-        <f>0</f>
-        <v>0</v>
-      </c>
-      <c r="F7" s="2">
+      <c r="E7" s="1">
+        <f>0</f>
+        <v>0</v>
+      </c>
+      <c r="F7" s="1">
         <f t="shared" si="2"/>
         <v>2.75</v>
       </c>
-    </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="G7" s="1"/>
+      <c r="H7" s="1"/>
+      <c r="I7" s="1"/>
+      <c r="J7" s="1"/>
+      <c r="K7" s="1"/>
+      <c r="L7" s="1"/>
+    </row>
+    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A8" s="1">
         <v>45219</v>
       </c>
-      <c r="B8" s="2">
+      <c r="B8" s="1">
         <f>1/6</f>
         <v>0.16666666666666666</v>
       </c>
-      <c r="C8" s="2">
+      <c r="C8" s="1">
         <f>1/6+1/3</f>
         <v>0.5</v>
       </c>
-      <c r="D8" s="2">
-        <f>0</f>
-        <v>0</v>
-      </c>
-      <c r="E8" s="2">
-        <f>0</f>
-        <v>0</v>
-      </c>
-      <c r="F8" s="2">
+      <c r="D8" s="1">
+        <f>0</f>
+        <v>0</v>
+      </c>
+      <c r="E8" s="1">
+        <f>0</f>
+        <v>0</v>
+      </c>
+      <c r="F8" s="1">
         <f t="shared" si="2"/>
         <v>0.66666666666666663</v>
       </c>
-    </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="G8" s="1"/>
+      <c r="H8" s="1"/>
+      <c r="I8" s="1"/>
+      <c r="J8" s="1"/>
+      <c r="K8" s="1"/>
+      <c r="L8" s="1"/>
+    </row>
+    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A9" s="1">
         <v>45220</v>
       </c>
-      <c r="B9" s="2">
-        <f>0</f>
-        <v>0</v>
-      </c>
-      <c r="C9" s="2">
+      <c r="B9" s="1">
+        <f>0</f>
+        <v>0</v>
+      </c>
+      <c r="C9" s="1">
         <f>22/60+1/6</f>
         <v>0.53333333333333333</v>
       </c>
-      <c r="D9" s="2">
-        <f>0</f>
-        <v>0</v>
-      </c>
-      <c r="E9" s="2">
-        <f>0</f>
-        <v>0</v>
-      </c>
-      <c r="F9" s="2">
+      <c r="D9" s="1">
+        <f>0</f>
+        <v>0</v>
+      </c>
+      <c r="E9" s="1">
+        <f>0</f>
+        <v>0</v>
+      </c>
+      <c r="F9" s="1">
         <f t="shared" si="2"/>
         <v>0.53333333333333333</v>
       </c>
-    </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="G9" s="1"/>
+      <c r="H9" s="1"/>
+      <c r="I9" s="1"/>
+      <c r="J9" s="1"/>
+      <c r="K9" s="1"/>
+      <c r="L9" s="1"/>
+    </row>
+    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A10" s="1">
         <v>45222</v>
       </c>
-      <c r="B10" s="2">
-        <f>0</f>
-        <v>0</v>
-      </c>
-      <c r="C10" s="2">
+      <c r="B10" s="1">
+        <f>0</f>
+        <v>0</v>
+      </c>
+      <c r="C10" s="1">
         <f>1/60*(22+22+22)</f>
         <v>1.1000000000000001</v>
       </c>
-      <c r="D10" s="2">
+      <c r="D10" s="1">
         <f>2/3</f>
         <v>0.66666666666666663</v>
       </c>
-      <c r="E10" s="2">
-        <f>0</f>
-        <v>0</v>
-      </c>
-      <c r="F10" s="2">
+      <c r="E10" s="1">
+        <f>0</f>
+        <v>0</v>
+      </c>
+      <c r="F10" s="1">
         <f t="shared" si="2"/>
         <v>1.7666666666666666</v>
       </c>
-    </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="G10" s="1"/>
+      <c r="H10" s="1"/>
+      <c r="I10" s="1"/>
+      <c r="J10" s="1"/>
+      <c r="K10" s="1"/>
+      <c r="L10" s="1"/>
+    </row>
+    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A11" s="1">
         <v>45231</v>
       </c>
-      <c r="B11" s="2">
-        <f>0</f>
-        <v>0</v>
-      </c>
-      <c r="C11" s="2">
+      <c r="B11" s="1">
+        <f>0</f>
+        <v>0</v>
+      </c>
+      <c r="C11" s="1">
         <f>(53+22+22)/60</f>
         <v>1.6166666666666667</v>
       </c>
-      <c r="D11" s="2">
+      <c r="D11" s="1">
         <f>(2+11)/60</f>
         <v>0.21666666666666667</v>
       </c>
-      <c r="E11" s="2">
+      <c r="E11" s="1">
         <f>(11+11)/60</f>
         <v>0.36666666666666664</v>
       </c>
-      <c r="F11" s="2">
+      <c r="F11" s="1">
         <f t="shared" si="2"/>
         <v>2.2000000000000002</v>
       </c>
-    </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="G11" s="1"/>
+      <c r="H11" s="1"/>
+      <c r="I11" s="1"/>
+      <c r="J11" s="1"/>
+      <c r="K11" s="1"/>
+      <c r="L11" s="1"/>
+    </row>
+    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A12" s="1">
         <v>45232</v>
       </c>
-      <c r="B12" s="2">
+      <c r="B12" s="1">
         <f>1/60 *(19)</f>
         <v>0.31666666666666665</v>
       </c>
-      <c r="C12" s="2">
+      <c r="C12" s="1">
         <f>1/60 *(10+23+21+13)</f>
         <v>1.1166666666666667</v>
       </c>
-      <c r="D12" s="2">
+      <c r="D12" s="1">
         <f>1/60 *(8+27+20)</f>
         <v>0.91666666666666663</v>
       </c>
-      <c r="E12" s="2">
-        <f>0</f>
-        <v>0</v>
-      </c>
-      <c r="F12" s="2">
+      <c r="E12" s="1">
+        <f>0</f>
+        <v>0</v>
+      </c>
+      <c r="F12" s="1">
         <f t="shared" si="2"/>
         <v>2.35</v>
       </c>
-    </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="G12" s="1"/>
+      <c r="H12" s="1"/>
+      <c r="I12" s="1"/>
+      <c r="J12" s="1"/>
+      <c r="K12" s="1"/>
+      <c r="L12" s="1"/>
+    </row>
+    <row r="13" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A13" s="1">
         <v>45233</v>
       </c>
-      <c r="B13">
+      <c r="B13" s="1">
         <f>(1/60)*(0)</f>
         <v>0</v>
       </c>
-      <c r="C13">
+      <c r="C13" s="1">
         <f>(1/60)*(21+21+21+21+21+21+15)</f>
         <v>2.35</v>
       </c>
-      <c r="D13">
-        <f t="shared" ref="C13:E13" si="3">(1/60)*(0)</f>
-        <v>0</v>
-      </c>
-      <c r="E13">
+      <c r="D13" s="1">
+        <f t="shared" ref="D13:E14" si="3">(1/60)*(0)</f>
+        <v>0</v>
+      </c>
+      <c r="E13" s="1">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
-      <c r="F13" s="2">
+      <c r="F13" s="1">
         <f t="shared" si="2"/>
         <v>2.35</v>
       </c>
-    </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G13" s="1"/>
+      <c r="H13" s="1"/>
+      <c r="I13" s="1"/>
+      <c r="J13" s="1"/>
+      <c r="K13" s="1"/>
+      <c r="L13" s="1"/>
+    </row>
+    <row r="14" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A14" s="1">
+        <v>45257</v>
+      </c>
+      <c r="B14" s="1">
+        <f>(1/60)*(5)</f>
+        <v>8.3333333333333329E-2</v>
+      </c>
+      <c r="C14" s="1">
+        <f>(1/60)*(21+16+21+10+6)</f>
+        <v>1.2333333333333334</v>
+      </c>
+      <c r="D14" s="1">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="E14" s="1">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="F14" s="1">
+        <f t="shared" si="2"/>
+        <v>1.3166666666666667</v>
+      </c>
+      <c r="G14" s="1"/>
+      <c r="H14" s="1"/>
+      <c r="I14" s="1"/>
+      <c r="J14" s="1"/>
+      <c r="K14" s="1"/>
+      <c r="L14" s="1"/>
+    </row>
+    <row r="15" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A15" s="1"/>
+      <c r="B15" s="1"/>
+      <c r="C15" s="1"/>
+      <c r="D15" s="1"/>
+      <c r="E15" s="1"/>
+      <c r="F15" s="1"/>
+      <c r="G15" s="1"/>
+      <c r="H15" s="1"/>
+      <c r="I15" s="1"/>
+      <c r="J15" s="1"/>
+      <c r="K15" s="1"/>
+      <c r="L15" s="1"/>
+    </row>
+    <row r="16" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A16" s="1"/>
+      <c r="B16" s="1"/>
+      <c r="C16" s="1"/>
+      <c r="D16" s="1"/>
+      <c r="E16" s="1"/>
+      <c r="F16" s="1"/>
+      <c r="G16" s="1"/>
+      <c r="H16" s="1"/>
+      <c r="I16" s="1"/>
+      <c r="J16" s="1"/>
+      <c r="K16" s="1"/>
+      <c r="L16" s="1"/>
+    </row>
+    <row r="17" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A17" s="1"/>
-      <c r="B17" s="2"/>
-      <c r="C17" s="2"/>
-      <c r="D17" s="2"/>
-      <c r="E17" s="2"/>
-      <c r="F17" s="2"/>
-    </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B17" s="1"/>
+      <c r="C17" s="1"/>
+      <c r="D17" s="1"/>
+      <c r="E17" s="1"/>
+      <c r="F17" s="1"/>
+      <c r="G17" s="1"/>
+      <c r="H17" s="1"/>
+      <c r="I17" s="1"/>
+      <c r="J17" s="1"/>
+      <c r="K17" s="1"/>
+      <c r="L17" s="1"/>
+    </row>
+    <row r="18" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A18" s="1"/>
-      <c r="B18" s="2"/>
-      <c r="C18" s="2"/>
-      <c r="D18" s="2"/>
-      <c r="E18" s="2"/>
-      <c r="F18" s="2"/>
-    </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B18" s="1"/>
+      <c r="C18" s="1"/>
+      <c r="D18" s="1"/>
+      <c r="E18" s="1"/>
+      <c r="F18" s="1"/>
+      <c r="G18" s="1"/>
+      <c r="H18" s="1"/>
+      <c r="I18" s="1"/>
+      <c r="J18" s="1"/>
+      <c r="K18" s="1"/>
+      <c r="L18" s="1"/>
+    </row>
+    <row r="19" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A19" s="1"/>
-      <c r="B19" s="2"/>
-      <c r="C19" s="2"/>
-      <c r="D19" s="2"/>
-      <c r="E19" s="2"/>
-      <c r="F19" s="2"/>
-    </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B19" s="1"/>
+      <c r="C19" s="1"/>
+      <c r="D19" s="1"/>
+      <c r="E19" s="1"/>
+      <c r="F19" s="1"/>
+      <c r="G19" s="1"/>
+      <c r="H19" s="1"/>
+      <c r="I19" s="1"/>
+      <c r="J19" s="1"/>
+      <c r="K19" s="1"/>
+      <c r="L19" s="1"/>
+    </row>
+    <row r="20" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A20" s="1"/>
-      <c r="B20" s="2"/>
-      <c r="C20" s="2"/>
-      <c r="D20" s="2"/>
-      <c r="E20" s="2"/>
-      <c r="F20" s="2"/>
-    </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B20" s="1"/>
+      <c r="C20" s="1"/>
+      <c r="D20" s="1"/>
+      <c r="E20" s="1"/>
+      <c r="F20" s="1"/>
+      <c r="G20" s="1"/>
+      <c r="H20" s="1"/>
+      <c r="I20" s="1"/>
+      <c r="J20" s="1"/>
+      <c r="K20" s="1"/>
+      <c r="L20" s="1"/>
+    </row>
+    <row r="21" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A21" s="1"/>
-      <c r="B21" s="2"/>
-      <c r="C21" s="2"/>
-      <c r="D21" s="2"/>
-      <c r="E21" s="2"/>
-      <c r="F21" s="2"/>
-    </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B21" s="1"/>
+      <c r="C21" s="1"/>
+      <c r="D21" s="1"/>
+      <c r="E21" s="1"/>
+      <c r="F21" s="1"/>
+      <c r="G21" s="1"/>
+      <c r="H21" s="1"/>
+      <c r="I21" s="1"/>
+      <c r="J21" s="1"/>
+      <c r="K21" s="1"/>
+      <c r="L21" s="1"/>
+    </row>
+    <row r="22" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A22" s="1"/>
-      <c r="B22" s="2"/>
-      <c r="C22" s="2"/>
-      <c r="D22" s="2"/>
-      <c r="E22" s="2"/>
-      <c r="F22" s="2"/>
-    </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B22" s="1"/>
+      <c r="C22" s="1"/>
+      <c r="D22" s="1"/>
+      <c r="E22" s="1"/>
+      <c r="F22" s="1"/>
+      <c r="G22" s="1"/>
+      <c r="H22" s="1"/>
+      <c r="I22" s="1"/>
+      <c r="J22" s="1"/>
+      <c r="K22" s="1"/>
+      <c r="L22" s="1"/>
+    </row>
+    <row r="23" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A23" s="1"/>
-      <c r="B23" s="2"/>
-      <c r="C23" s="2"/>
-      <c r="D23" s="2"/>
-      <c r="E23" s="2"/>
-      <c r="F23" s="2"/>
+      <c r="B23" s="1"/>
+      <c r="C23" s="1"/>
+      <c r="D23" s="1"/>
+      <c r="E23" s="1"/>
+      <c r="F23" s="1"/>
+      <c r="G23" s="1"/>
+      <c r="H23" s="1"/>
+      <c r="I23" s="1"/>
+      <c r="J23" s="1"/>
+      <c r="K23" s="1"/>
+      <c r="L23" s="1"/>
+    </row>
+    <row r="24" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A24" s="1"/>
+      <c r="B24" s="1"/>
+      <c r="C24" s="1"/>
+      <c r="D24" s="1"/>
+      <c r="E24" s="1"/>
+      <c r="F24" s="1"/>
+      <c r="G24" s="1"/>
+      <c r="H24" s="1"/>
+      <c r="I24" s="1"/>
+      <c r="J24" s="1"/>
+      <c r="K24" s="1"/>
+      <c r="L24" s="1"/>
+    </row>
+    <row r="25" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A25" s="1"/>
+      <c r="B25" s="1"/>
+      <c r="C25" s="1"/>
+      <c r="D25" s="1"/>
+      <c r="E25" s="1"/>
+      <c r="F25" s="1"/>
+      <c r="G25" s="1"/>
+      <c r="H25" s="1"/>
+      <c r="I25" s="1"/>
+      <c r="J25" s="1"/>
+      <c r="K25" s="1"/>
+      <c r="L25" s="1"/>
+    </row>
+    <row r="26" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A26" s="1"/>
+      <c r="B26" s="1"/>
+      <c r="C26" s="1"/>
+      <c r="D26" s="1"/>
+      <c r="E26" s="1"/>
+      <c r="F26" s="1"/>
+      <c r="G26" s="1"/>
+      <c r="H26" s="1"/>
+      <c r="I26" s="1"/>
+      <c r="J26" s="1"/>
+      <c r="K26" s="1"/>
+      <c r="L26" s="1"/>
+    </row>
+    <row r="27" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A27" s="1"/>
+      <c r="B27" s="1"/>
+      <c r="C27" s="1"/>
+      <c r="D27" s="1"/>
+      <c r="E27" s="1"/>
+      <c r="F27" s="1"/>
+      <c r="G27" s="1"/>
+      <c r="H27" s="1"/>
+      <c r="I27" s="1"/>
+      <c r="J27" s="1"/>
+      <c r="K27" s="1"/>
+      <c r="L27" s="1"/>
+    </row>
+    <row r="28" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A28" s="1"/>
+      <c r="B28" s="1"/>
+      <c r="C28" s="1"/>
+      <c r="D28" s="1"/>
+      <c r="E28" s="1"/>
+      <c r="F28" s="1"/>
+      <c r="G28" s="1"/>
+      <c r="H28" s="1"/>
+      <c r="I28" s="1"/>
+      <c r="J28" s="1"/>
+      <c r="K28" s="1"/>
+      <c r="L28" s="1"/>
+    </row>
+    <row r="29" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A29" s="1"/>
+      <c r="B29" s="1"/>
+      <c r="C29" s="1"/>
+      <c r="D29" s="1"/>
+      <c r="E29" s="1"/>
+      <c r="F29" s="1"/>
+      <c r="G29" s="1"/>
+      <c r="H29" s="1"/>
+      <c r="I29" s="1"/>
+      <c r="J29" s="1"/>
+      <c r="K29" s="1"/>
+      <c r="L29" s="1"/>
+    </row>
+    <row r="30" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A30" s="1"/>
+      <c r="B30" s="1"/>
+      <c r="C30" s="1"/>
+      <c r="D30" s="1"/>
+      <c r="E30" s="1"/>
+      <c r="F30" s="1"/>
+      <c r="G30" s="1"/>
+      <c r="H30" s="1"/>
+      <c r="I30" s="1"/>
+      <c r="J30" s="1"/>
+      <c r="K30" s="1"/>
+      <c r="L30" s="1"/>
+    </row>
+    <row r="31" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A31" s="1"/>
+      <c r="B31" s="1"/>
+      <c r="C31" s="1"/>
+      <c r="D31" s="1"/>
+      <c r="E31" s="1"/>
+      <c r="F31" s="1"/>
+      <c r="G31" s="1"/>
+      <c r="H31" s="1"/>
+      <c r="I31" s="1"/>
+      <c r="J31" s="1"/>
+      <c r="K31" s="1"/>
+      <c r="L31" s="1"/>
+    </row>
+    <row r="32" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A32" s="1"/>
+      <c r="B32" s="1"/>
+      <c r="C32" s="1"/>
+      <c r="D32" s="1"/>
+      <c r="E32" s="1"/>
+      <c r="F32" s="1"/>
+      <c r="G32" s="1"/>
+      <c r="H32" s="1"/>
+      <c r="I32" s="1"/>
+      <c r="J32" s="1"/>
+      <c r="K32" s="1"/>
+      <c r="L32" s="1"/>
+    </row>
+    <row r="33" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A33" s="1"/>
+      <c r="B33" s="1"/>
+      <c r="C33" s="1"/>
+      <c r="D33" s="1"/>
+      <c r="E33" s="1"/>
+      <c r="F33" s="1"/>
+      <c r="G33" s="1"/>
+      <c r="H33" s="1"/>
+      <c r="I33" s="1"/>
+      <c r="J33" s="1"/>
+      <c r="K33" s="1"/>
+      <c r="L33" s="1"/>
+    </row>
+    <row r="34" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A34" s="1"/>
+      <c r="B34" s="1"/>
+      <c r="C34" s="1"/>
+      <c r="D34" s="1"/>
+      <c r="E34" s="1"/>
+      <c r="F34" s="1"/>
+      <c r="G34" s="1"/>
+      <c r="H34" s="1"/>
+      <c r="I34" s="1"/>
+      <c r="J34" s="1"/>
+      <c r="K34" s="1"/>
+      <c r="L34" s="1"/>
+    </row>
+    <row r="35" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A35" s="1"/>
+      <c r="B35" s="1"/>
+      <c r="C35" s="1"/>
+      <c r="D35" s="1"/>
+      <c r="E35" s="1"/>
+      <c r="F35" s="1"/>
+      <c r="G35" s="1"/>
+      <c r="H35" s="1"/>
+      <c r="I35" s="1"/>
+      <c r="J35" s="1"/>
+      <c r="K35" s="1"/>
+      <c r="L35" s="1"/>
+    </row>
+    <row r="36" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A36" s="1"/>
+      <c r="B36" s="1"/>
+      <c r="C36" s="1"/>
+      <c r="D36" s="1"/>
+      <c r="E36" s="1"/>
+      <c r="F36" s="1"/>
+      <c r="G36" s="1"/>
+      <c r="H36" s="1"/>
+      <c r="I36" s="1"/>
+      <c r="J36" s="1"/>
+      <c r="K36" s="1"/>
+      <c r="L36" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
whyy am i so bad
</commit_message>
<xml_diff>
--- a/Docs/timesheet.xlsx
+++ b/Docs/timesheet.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Alex\Documents\School\Y2\Personal Portfolio\pp2\UnrealEngineBasics\Docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CE4D57CD-EA13-4BC0-A7FB-A2BDFB337DE7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{26296888-1374-4B8A-822C-2647C77FBB1F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-28920" yWindow="-105" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -404,7 +404,7 @@
   <dimension ref="A1:L36"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C18" sqref="C18"/>
+      <selection activeCell="C19" sqref="C19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -485,7 +485,7 @@
       </c>
       <c r="C3" s="1">
         <f>SUM(C5:C32)</f>
-        <v>12.666666666666666</v>
+        <v>12.983333333333333</v>
       </c>
       <c r="D3" s="1">
         <f>SUM(D5:D32)</f>
@@ -497,7 +497,7 @@
       </c>
       <c r="F3" s="1">
         <f>SUM(B3:E3)</f>
-        <v>21.016666666666669</v>
+        <v>21.333333333333332</v>
       </c>
       <c r="G3" s="1">
         <f>(1/60)*(180+20+10)</f>
@@ -505,7 +505,7 @@
       </c>
       <c r="H3" s="1">
         <f>F3+G3</f>
-        <v>24.516666666666669</v>
+        <v>24.833333333333332</v>
       </c>
       <c r="I3" s="1"/>
       <c r="J3" s="1"/>
@@ -522,7 +522,7 @@
       </c>
       <c r="C4" s="2">
         <f t="shared" ref="C4:E4" si="1">(C3/C2)</f>
-        <v>0.42222222222222222</v>
+        <v>0.43277777777777776</v>
       </c>
       <c r="D4" s="2">
         <f t="shared" si="1"/>
@@ -534,12 +534,12 @@
       </c>
       <c r="F4" s="2">
         <f>(F3/F2)</f>
-        <v>0.26270833333333338</v>
+        <v>0.26666666666666666</v>
       </c>
       <c r="G4" s="1"/>
       <c r="H4" s="2">
         <f>(H3/F2)</f>
-        <v>0.30645833333333339</v>
+        <v>0.31041666666666667</v>
       </c>
       <c r="I4" s="1"/>
       <c r="J4" s="1"/>
@@ -945,14 +945,16 @@
       <c r="L17" s="1"/>
     </row>
     <row r="18" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A18" s="4"/>
+      <c r="A18" s="4">
+        <v>45272</v>
+      </c>
       <c r="B18" s="1">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="C18" s="1">
-        <f t="shared" si="3"/>
-        <v>0</v>
+        <f>(1/60)*(19)</f>
+        <v>0.31666666666666665</v>
       </c>
       <c r="D18" s="1">
         <f t="shared" si="3"/>
@@ -964,7 +966,7 @@
       </c>
       <c r="F18" s="1">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>0.31666666666666665</v>
       </c>
       <c r="G18" s="1"/>
       <c r="H18" s="1"/>

</xml_diff>

<commit_message>
punch animation fix (blend animation)
</commit_message>
<xml_diff>
--- a/Docs/timesheet.xlsx
+++ b/Docs/timesheet.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Alex\Documents\School\Y2\Personal Portfolio\pp2\UnrealEngineBasics\Docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9B525E26-923A-4FC4-AFB8-70A53CE43CFC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6129EFB2-1660-44AA-994E-260FD09BF1AA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-28920" yWindow="-105" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -404,7 +404,7 @@
   <dimension ref="A1:L36"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C20" sqref="C20"/>
+      <selection activeCell="F22" sqref="F22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -481,7 +481,7 @@
       </c>
       <c r="B3" s="1">
         <f>SUM(B5:B23)</f>
-        <v>3.4333333333333336</v>
+        <v>3.5166666666666671</v>
       </c>
       <c r="C3" s="1">
         <f>SUM(C5:C32)</f>
@@ -489,7 +489,7 @@
       </c>
       <c r="D3" s="1">
         <f>SUM(D5:D32)</f>
-        <v>4.55</v>
+        <v>4.8</v>
       </c>
       <c r="E3" s="1">
         <f>SUM(E5:E32)</f>
@@ -497,7 +497,7 @@
       </c>
       <c r="F3" s="1">
         <f>SUM(B3:E3)</f>
-        <v>26.5</v>
+        <v>26.833333333333332</v>
       </c>
       <c r="G3" s="1">
         <f>(1/60)*(180+20+10)</f>
@@ -505,7 +505,7 @@
       </c>
       <c r="H3" s="1">
         <f>F3+G3</f>
-        <v>30</v>
+        <v>30.333333333333332</v>
       </c>
       <c r="I3" s="1"/>
       <c r="J3" s="1"/>
@@ -518,7 +518,7 @@
       </c>
       <c r="B4" s="2">
         <f>(B3/B2)</f>
-        <v>0.34333333333333338</v>
+        <v>0.35166666666666668</v>
       </c>
       <c r="C4" s="2">
         <f t="shared" ref="C4:E4" si="1">(C3/C2)</f>
@@ -526,7 +526,7 @@
       </c>
       <c r="D4" s="2">
         <f t="shared" si="1"/>
-        <v>0.45499999999999996</v>
+        <v>0.48</v>
       </c>
       <c r="E4" s="2">
         <f t="shared" si="1"/>
@@ -534,12 +534,12 @@
       </c>
       <c r="F4" s="2">
         <f>(F3/F2)</f>
-        <v>0.33124999999999999</v>
+        <v>0.33541666666666664</v>
       </c>
       <c r="G4" s="1"/>
       <c r="H4" s="2">
         <f>(H3/F2)</f>
-        <v>0.375</v>
+        <v>0.37916666666666665</v>
       </c>
       <c r="I4" s="1"/>
       <c r="J4" s="1"/>
@@ -566,7 +566,7 @@
         <v>0</v>
       </c>
       <c r="F5" s="1">
-        <f t="shared" ref="F5:F21" si="2">SUM(B5:E5)</f>
+        <f t="shared" ref="F5:F22" si="2">SUM(B5:E5)</f>
         <v>1</v>
       </c>
       <c r="G5" s="1"/>
@@ -802,7 +802,7 @@
         <v>2.35</v>
       </c>
       <c r="D13" s="1">
-        <f t="shared" ref="B13:E21" si="3">(1/60)*(0)</f>
+        <f t="shared" ref="B13:F22" si="3">(1/60)*(0)</f>
         <v>0</v>
       </c>
       <c r="E13" s="1">
@@ -1038,18 +1038,20 @@
       <c r="L20" s="1"/>
     </row>
     <row r="21" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A21" s="4"/>
+      <c r="A21" s="4">
+        <v>45280</v>
+      </c>
       <c r="B21" s="1">
-        <f t="shared" si="3"/>
-        <v>0</v>
+        <f>(1/60)*(5)</f>
+        <v>8.3333333333333329E-2</v>
       </c>
       <c r="C21" s="1">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="D21" s="1">
-        <f t="shared" si="3"/>
-        <v>0</v>
+        <f>(1/60)*(15)</f>
+        <v>0.25</v>
       </c>
       <c r="E21" s="1">
         <f t="shared" si="3"/>
@@ -1057,7 +1059,7 @@
       </c>
       <c r="F21" s="1">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>0.33333333333333331</v>
       </c>
       <c r="G21" s="1"/>
       <c r="H21" s="1"/>
@@ -1068,11 +1070,26 @@
     </row>
     <row r="22" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A22" s="4"/>
-      <c r="B22" s="1"/>
-      <c r="C22" s="1"/>
-      <c r="D22" s="1"/>
-      <c r="E22" s="1"/>
-      <c r="F22" s="1"/>
+      <c r="B22" s="1">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="C22" s="1">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="D22" s="1">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="E22" s="1">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="F22" s="1">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
       <c r="G22" s="1"/>
       <c r="H22" s="1"/>
       <c r="I22" s="1"/>

</xml_diff>

<commit_message>
find nearest enemy start
</commit_message>
<xml_diff>
--- a/Docs/timesheet.xlsx
+++ b/Docs/timesheet.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Alex\Documents\School\Y2\Personal Portfolio\pp2\UnrealEngineBasics\Docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{85987A7B-6485-4A54-B9B2-CDA332556E3F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C3B155AD-C2FC-48AF-B0AF-86D2A5AE83E9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-28920" yWindow="-105" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -62,13 +62,13 @@
     <t>Total</t>
   </si>
   <si>
-    <t>Documentation</t>
-  </si>
-  <si>
     <t>Total+Doc</t>
   </si>
   <si>
     <t>Percentage:</t>
+  </si>
+  <si>
+    <t>Documentation/etc</t>
   </si>
 </sst>
 </file>
@@ -405,7 +405,7 @@
   <dimension ref="A1:L36"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B28" sqref="B28"/>
+      <selection activeCell="H12" sqref="H12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -416,7 +416,7 @@
     <col min="4" max="4" width="25.42578125" customWidth="1"/>
     <col min="5" max="5" width="24.28515625" customWidth="1"/>
     <col min="6" max="6" width="9.140625" customWidth="1"/>
-    <col min="7" max="7" width="15.28515625" customWidth="1"/>
+    <col min="7" max="7" width="23.5703125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:12" x14ac:dyDescent="0.25">
@@ -439,10 +439,10 @@
         <v>7</v>
       </c>
       <c r="G1" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="H1" s="3" t="s">
         <v>8</v>
-      </c>
-      <c r="H1" s="3" t="s">
-        <v>9</v>
       </c>
       <c r="I1" s="1"/>
       <c r="J1" s="1"/>
@@ -494,19 +494,19 @@
       </c>
       <c r="E3" s="1">
         <f>SUM(E5:E32)</f>
-        <v>3.0833333333333335</v>
+        <v>3.416666666666667</v>
       </c>
       <c r="F3" s="1">
         <f>SUM(B3:E3)</f>
-        <v>34.783333333333331</v>
+        <v>35.11666666666666</v>
       </c>
       <c r="G3" s="1">
-        <f>(1/60)*(180+20+10)</f>
-        <v>3.5</v>
+        <f>(1/60)*(180+20+10+6)</f>
+        <v>3.6</v>
       </c>
       <c r="H3" s="1">
         <f>F3+G3</f>
-        <v>38.283333333333331</v>
+        <v>38.716666666666661</v>
       </c>
       <c r="I3" s="1"/>
       <c r="J3" s="1"/>
@@ -515,7 +515,7 @@
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B4" s="2">
         <f>(B3/B2)</f>
@@ -531,16 +531,16 @@
       </c>
       <c r="E4" s="2">
         <f t="shared" si="1"/>
-        <v>0.10277777777777779</v>
+        <v>0.1138888888888889</v>
       </c>
       <c r="F4" s="2">
         <f>(F3/F2)</f>
-        <v>0.43479166666666663</v>
+        <v>0.43895833333333323</v>
       </c>
       <c r="G4" s="1"/>
       <c r="H4" s="2">
         <f>(H3/F2)</f>
-        <v>0.47854166666666664</v>
+        <v>0.48395833333333327</v>
       </c>
       <c r="I4" s="1"/>
       <c r="J4" s="1"/>
@@ -1241,12 +1241,12 @@
         <v>8.3333333333333329E-2</v>
       </c>
       <c r="E27" s="1">
-        <f>(1/60)*(21+26+20)</f>
-        <v>1.1166666666666667</v>
+        <f>(1/60)*(21+26+20+20)</f>
+        <v>1.45</v>
       </c>
       <c r="F27" s="1">
         <f t="shared" ref="F27" si="8">SUM(B27:E27)</f>
-        <v>1.3</v>
+        <v>1.6333333333333333</v>
       </c>
       <c r="G27" s="1"/>
       <c r="H27" s="1"/>

</xml_diff>

<commit_message>
homing + target assist missiles.
enemies can be dmged
</commit_message>
<xml_diff>
--- a/Docs/timesheet.xlsx
+++ b/Docs/timesheet.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Alex\Documents\School\Y2\Personal Portfolio\pp2\UnrealEngineBasics\Docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C3B155AD-C2FC-48AF-B0AF-86D2A5AE83E9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{51209CB8-45FF-4075-86EE-1538C99E9C17}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-28920" yWindow="-105" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -405,7 +405,7 @@
   <dimension ref="A1:L36"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H12" sqref="H12"/>
+      <selection activeCell="D27" sqref="D27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -486,7 +486,7 @@
       </c>
       <c r="C3" s="1">
         <f>SUM(C5:C32)</f>
-        <v>18.666666666666664</v>
+        <v>18.749999999999996</v>
       </c>
       <c r="D3" s="1">
         <f>SUM(D5:D32)</f>
@@ -494,11 +494,11 @@
       </c>
       <c r="E3" s="1">
         <f>SUM(E5:E32)</f>
-        <v>3.416666666666667</v>
+        <v>4.5333333333333332</v>
       </c>
       <c r="F3" s="1">
         <f>SUM(B3:E3)</f>
-        <v>35.11666666666666</v>
+        <v>36.316666666666663</v>
       </c>
       <c r="G3" s="1">
         <f>(1/60)*(180+20+10+6)</f>
@@ -506,7 +506,7 @@
       </c>
       <c r="H3" s="1">
         <f>F3+G3</f>
-        <v>38.716666666666661</v>
+        <v>39.916666666666664</v>
       </c>
       <c r="I3" s="1"/>
       <c r="J3" s="1"/>
@@ -523,7 +523,7 @@
       </c>
       <c r="C4" s="2">
         <f t="shared" ref="C4:E4" si="1">(C3/C2)</f>
-        <v>0.62222222222222212</v>
+        <v>0.62499999999999989</v>
       </c>
       <c r="D4" s="2">
         <f t="shared" si="1"/>
@@ -531,16 +531,16 @@
       </c>
       <c r="E4" s="2">
         <f t="shared" si="1"/>
-        <v>0.1138888888888889</v>
+        <v>0.15111111111111111</v>
       </c>
       <c r="F4" s="2">
         <f>(F3/F2)</f>
-        <v>0.43895833333333323</v>
+        <v>0.4539583333333333</v>
       </c>
       <c r="G4" s="1"/>
       <c r="H4" s="2">
         <f>(H3/F2)</f>
-        <v>0.48395833333333327</v>
+        <v>0.49895833333333328</v>
       </c>
       <c r="I4" s="1"/>
       <c r="J4" s="1"/>
@@ -1229,24 +1229,24 @@
         <v>45310</v>
       </c>
       <c r="B27" s="1">
-        <f>(1/60)*(6)</f>
-        <v>0.1</v>
+        <f>(1/60)*(6+6)</f>
+        <v>0.2</v>
       </c>
       <c r="C27" s="1">
-        <f t="shared" si="3"/>
-        <v>0</v>
+        <f>(1/60)*(5)</f>
+        <v>8.3333333333333329E-2</v>
       </c>
       <c r="D27" s="1">
         <f>(1/60)*(5)</f>
         <v>8.3333333333333329E-2</v>
       </c>
       <c r="E27" s="1">
-        <f>(1/60)*(21+26+20+20)</f>
-        <v>1.45</v>
+        <f>(1/60)*(21+26+20+20+26+26+15)</f>
+        <v>2.5666666666666664</v>
       </c>
       <c r="F27" s="1">
         <f t="shared" ref="F27" si="8">SUM(B27:E27)</f>
-        <v>1.6333333333333333</v>
+        <v>2.9333333333333331</v>
       </c>
       <c r="G27" s="1"/>
       <c r="H27" s="1"/>

</xml_diff>

<commit_message>
switch chars + switch spells beg, new walk anim (rifle)
</commit_message>
<xml_diff>
--- a/Docs/timesheet.xlsx
+++ b/Docs/timesheet.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Alex\Documents\School\Y2\Personal Portfolio\pp2\UnrealEngineBasics\Docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{51209CB8-45FF-4075-86EE-1538C99E9C17}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B5E753AD-ACE8-49BC-B5E9-8ECFDC7C8C5E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-28920" yWindow="-105" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -405,7 +405,7 @@
   <dimension ref="A1:L36"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D27" sqref="D27"/>
+      <selection activeCell="C29" sqref="C29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -486,11 +486,11 @@
       </c>
       <c r="C3" s="1">
         <f>SUM(C5:C32)</f>
-        <v>18.749999999999996</v>
+        <v>18.799999999999997</v>
       </c>
       <c r="D3" s="1">
         <f>SUM(D5:D32)</f>
-        <v>9.5166666666666675</v>
+        <v>9.7666666666666675</v>
       </c>
       <c r="E3" s="1">
         <f>SUM(E5:E32)</f>
@@ -498,7 +498,7 @@
       </c>
       <c r="F3" s="1">
         <f>SUM(B3:E3)</f>
-        <v>36.316666666666663</v>
+        <v>36.61666666666666</v>
       </c>
       <c r="G3" s="1">
         <f>(1/60)*(180+20+10+6)</f>
@@ -506,7 +506,7 @@
       </c>
       <c r="H3" s="1">
         <f>F3+G3</f>
-        <v>39.916666666666664</v>
+        <v>40.216666666666661</v>
       </c>
       <c r="I3" s="1"/>
       <c r="J3" s="1"/>
@@ -523,11 +523,11 @@
       </c>
       <c r="C4" s="2">
         <f t="shared" ref="C4:E4" si="1">(C3/C2)</f>
-        <v>0.62499999999999989</v>
+        <v>0.62666666666666659</v>
       </c>
       <c r="D4" s="2">
         <f t="shared" si="1"/>
-        <v>0.95166666666666677</v>
+        <v>0.97666666666666679</v>
       </c>
       <c r="E4" s="2">
         <f t="shared" si="1"/>
@@ -535,12 +535,12 @@
       </c>
       <c r="F4" s="2">
         <f>(F3/F2)</f>
-        <v>0.4539583333333333</v>
+        <v>0.45770833333333327</v>
       </c>
       <c r="G4" s="1"/>
       <c r="H4" s="2">
         <f>(H3/F2)</f>
-        <v>0.49895833333333328</v>
+        <v>0.50270833333333331</v>
       </c>
       <c r="I4" s="1"/>
       <c r="J4" s="1"/>
@@ -803,7 +803,7 @@
         <v>2.35</v>
       </c>
       <c r="D13" s="1">
-        <f t="shared" ref="B13:E28" si="3">(1/60)*(0)</f>
+        <f t="shared" ref="B13:E29" si="3">(1/60)*(0)</f>
         <v>0</v>
       </c>
       <c r="E13" s="1">
@@ -1245,7 +1245,7 @@
         <v>2.5666666666666664</v>
       </c>
       <c r="F27" s="1">
-        <f t="shared" ref="F27" si="8">SUM(B27:E27)</f>
+        <f t="shared" ref="F27:F28" si="8">SUM(B27:E27)</f>
         <v>2.9333333333333331</v>
       </c>
       <c r="G27" s="1"/>
@@ -1256,24 +1256,29 @@
       <c r="L27" s="1"/>
     </row>
     <row r="28" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A28" s="1"/>
+      <c r="A28" s="4">
+        <v>45314</v>
+      </c>
       <c r="B28" s="1">
-        <f t="shared" si="3"/>
-        <v>0</v>
+        <f>(1/60)*(8)</f>
+        <v>0.13333333333333333</v>
       </c>
       <c r="C28" s="1">
-        <f t="shared" si="3"/>
-        <v>0</v>
+        <f>(1/60)*(3)</f>
+        <v>0.05</v>
       </c>
       <c r="D28" s="1">
-        <f>(1/60)*(0)</f>
-        <v>0</v>
+        <f>(1/60)*(15)</f>
+        <v>0.25</v>
       </c>
       <c r="E28" s="1">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
-      <c r="F28" s="1"/>
+      <c r="F28" s="1">
+        <f t="shared" si="8"/>
+        <v>0.43333333333333335</v>
+      </c>
       <c r="G28" s="1"/>
       <c r="H28" s="1"/>
       <c r="I28" s="1"/>
@@ -1282,12 +1287,29 @@
       <c r="L28" s="1"/>
     </row>
     <row r="29" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A29" s="1"/>
-      <c r="B29" s="1"/>
-      <c r="C29" s="1"/>
-      <c r="D29" s="1"/>
-      <c r="E29" s="1"/>
-      <c r="F29" s="1"/>
+      <c r="A29" s="4">
+        <v>45315</v>
+      </c>
+      <c r="B29" s="1">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="C29" s="1">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="D29" s="1">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="E29" s="1">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="F29" s="1">
+        <f t="shared" ref="F29" si="9">SUM(B29:E29)</f>
+        <v>0</v>
+      </c>
       <c r="G29" s="1"/>
       <c r="H29" s="1"/>
       <c r="I29" s="1"/>

</xml_diff>

<commit_message>
gun auto and burst + trigger cd
</commit_message>
<xml_diff>
--- a/Docs/timesheet.xlsx
+++ b/Docs/timesheet.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27126"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27029"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Alex\Documents\School\Y2\Personal Portfolio\pp2\UnrealEngineBasics\Docs\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Libraries\Documents\School\Y2\Personal Portfolio\pp2\UnrealEngineBasics\Docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5463AE86-22FB-40BD-A078-10EFB02A2189}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2C6E15DD-DA98-4C1E-9220-0747AEC34EFD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-105" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="3075" yWindow="3075" windowWidth="21600" windowHeight="11295" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -404,8 +404,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:L36"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E30" sqref="E30"/>
+    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="E31" sqref="E31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -494,11 +494,11 @@
       </c>
       <c r="E3" s="1">
         <f>SUM(E5:E32)</f>
-        <v>8.5500000000000007</v>
+        <v>9.8166666666666664</v>
       </c>
       <c r="F3" s="1">
         <f>SUM(B3:E3)</f>
-        <v>40.733333333333334</v>
+        <v>42</v>
       </c>
       <c r="G3" s="1">
         <f>(1/60)*(180+20+10+6)</f>
@@ -506,7 +506,7 @@
       </c>
       <c r="H3" s="1">
         <f>F3+G3</f>
-        <v>44.333333333333336</v>
+        <v>45.6</v>
       </c>
       <c r="I3" s="1"/>
       <c r="J3" s="1"/>
@@ -531,16 +531,16 @@
       </c>
       <c r="E4" s="2">
         <f t="shared" si="1"/>
-        <v>0.28500000000000003</v>
+        <v>0.32722222222222219</v>
       </c>
       <c r="F4" s="2">
         <f>(F3/F2)</f>
-        <v>0.50916666666666666</v>
+        <v>0.52500000000000002</v>
       </c>
       <c r="G4" s="1"/>
       <c r="H4" s="2">
         <f>(H3/F2)</f>
-        <v>0.5541666666666667</v>
+        <v>0.57000000000000006</v>
       </c>
       <c r="I4" s="1"/>
       <c r="J4" s="1"/>
@@ -803,7 +803,7 @@
         <v>2.35</v>
       </c>
       <c r="D13" s="1">
-        <f t="shared" ref="B13:E30" si="3">(1/60)*(0)</f>
+        <f t="shared" ref="B13:E31" si="3">(1/60)*(0)</f>
         <v>0</v>
       </c>
       <c r="E13" s="1">
@@ -1334,12 +1334,12 @@
         <v>0</v>
       </c>
       <c r="E30" s="1">
-        <f t="shared" si="3"/>
-        <v>0</v>
+        <f>(1/60)*(26+24+26)</f>
+        <v>1.2666666666666666</v>
       </c>
       <c r="F30" s="1">
         <f t="shared" ref="F30" si="10">SUM(B30:E30)</f>
-        <v>0</v>
+        <v>1.2666666666666666</v>
       </c>
       <c r="G30" s="1"/>
       <c r="H30" s="1"/>
@@ -1349,12 +1349,29 @@
       <c r="L30" s="1"/>
     </row>
     <row r="31" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A31" s="1"/>
-      <c r="B31" s="1"/>
-      <c r="C31" s="1"/>
-      <c r="D31" s="1"/>
-      <c r="E31" s="1"/>
-      <c r="F31" s="1"/>
+      <c r="A31" s="4">
+        <v>45318</v>
+      </c>
+      <c r="B31" s="1">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="C31" s="1">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="D31" s="1">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="E31" s="1">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="F31" s="1">
+        <f t="shared" ref="F31" si="11">SUM(B31:E31)</f>
+        <v>0</v>
+      </c>
       <c r="G31" s="1"/>
       <c r="H31" s="1"/>
       <c r="I31" s="1"/>

</xml_diff>

<commit_message>
UI change on char switch + invert cam possible
</commit_message>
<xml_diff>
--- a/Docs/timesheet.xlsx
+++ b/Docs/timesheet.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Alex\Documents\School\Y2\Personal Portfolio\pp2\UnrealEngineBasics\Docs\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Libraries\Documents\School\Y2\Personal Portfolio\pp2\UnrealEngineBasics\Docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0737A122-85F7-485D-A361-DE74C15FB325}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CDF2A62C-AA26-4D71-AE4C-BF17EC6B470E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-105" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -402,10 +402,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:L36"/>
+  <dimension ref="A1:L37"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E33" sqref="E33"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="B33" sqref="B33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -803,7 +803,7 @@
         <v>2.35</v>
       </c>
       <c r="D13" s="1">
-        <f t="shared" ref="B13:E33" si="3">(1/60)*(0)</f>
+        <f t="shared" ref="B13:E34" si="3">(1/60)*(0)</f>
         <v>0</v>
       </c>
       <c r="E13" s="1">
@@ -1411,14 +1411,16 @@
       <c r="L32" s="1"/>
     </row>
     <row r="33" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A33" s="1"/>
+      <c r="A33" s="4">
+        <v>45334</v>
+      </c>
       <c r="B33" s="1">
-        <f t="shared" si="3"/>
-        <v>0</v>
+        <f>(1/60)*(13)</f>
+        <v>0.21666666666666667</v>
       </c>
       <c r="C33" s="1">
-        <f t="shared" si="3"/>
-        <v>0</v>
+        <f>(1/60)*(21+8)</f>
+        <v>0.48333333333333334</v>
       </c>
       <c r="D33" s="1">
         <f t="shared" si="3"/>
@@ -1430,7 +1432,7 @@
       </c>
       <c r="F33" s="1">
         <f t="shared" ref="F33" si="13">SUM(B33:E33)</f>
-        <v>0</v>
+        <v>0.7</v>
       </c>
       <c r="G33" s="1"/>
       <c r="H33" s="1"/>
@@ -1440,12 +1442,29 @@
       <c r="L33" s="1"/>
     </row>
     <row r="34" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A34" s="1"/>
-      <c r="B34" s="1"/>
-      <c r="C34" s="1"/>
-      <c r="D34" s="1"/>
-      <c r="E34" s="1"/>
-      <c r="F34" s="1"/>
+      <c r="A34" s="4">
+        <v>45335</v>
+      </c>
+      <c r="B34" s="1">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="C34" s="1">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="D34" s="1">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="E34" s="1">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="F34" s="1">
+        <f t="shared" ref="F34:F37" si="14">SUM(B34:E34)</f>
+        <v>0</v>
+      </c>
       <c r="G34" s="1"/>
       <c r="H34" s="1"/>
       <c r="I34" s="1"/>
@@ -1454,12 +1473,29 @@
       <c r="L34" s="1"/>
     </row>
     <row r="35" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A35" s="1"/>
-      <c r="B35" s="1"/>
-      <c r="C35" s="1"/>
-      <c r="D35" s="1"/>
-      <c r="E35" s="1"/>
-      <c r="F35" s="1"/>
+      <c r="A35" s="4">
+        <v>45336</v>
+      </c>
+      <c r="B35" s="1">
+        <f t="shared" ref="B35:E37" si="15">(1/60)*(0)</f>
+        <v>0</v>
+      </c>
+      <c r="C35" s="1">
+        <f t="shared" si="15"/>
+        <v>0</v>
+      </c>
+      <c r="D35" s="1">
+        <f t="shared" si="15"/>
+        <v>0</v>
+      </c>
+      <c r="E35" s="1">
+        <f t="shared" si="15"/>
+        <v>0</v>
+      </c>
+      <c r="F35" s="1">
+        <f t="shared" si="14"/>
+        <v>0</v>
+      </c>
       <c r="G35" s="1"/>
       <c r="H35" s="1"/>
       <c r="I35" s="1"/>
@@ -1468,18 +1504,58 @@
       <c r="L35" s="1"/>
     </row>
     <row r="36" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A36" s="1"/>
-      <c r="B36" s="1"/>
-      <c r="C36" s="1"/>
-      <c r="D36" s="1"/>
-      <c r="E36" s="1"/>
-      <c r="F36" s="1"/>
+      <c r="A36" s="4">
+        <v>45337</v>
+      </c>
+      <c r="B36" s="1">
+        <f t="shared" si="15"/>
+        <v>0</v>
+      </c>
+      <c r="C36" s="1">
+        <f t="shared" si="15"/>
+        <v>0</v>
+      </c>
+      <c r="D36" s="1">
+        <f t="shared" si="15"/>
+        <v>0</v>
+      </c>
+      <c r="E36" s="1">
+        <f t="shared" si="15"/>
+        <v>0</v>
+      </c>
+      <c r="F36" s="1">
+        <f t="shared" si="14"/>
+        <v>0</v>
+      </c>
       <c r="G36" s="1"/>
       <c r="H36" s="1"/>
       <c r="I36" s="1"/>
       <c r="J36" s="1"/>
       <c r="K36" s="1"/>
       <c r="L36" s="1"/>
+    </row>
+    <row r="37" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A37" s="4"/>
+      <c r="B37" s="1">
+        <f t="shared" si="15"/>
+        <v>0</v>
+      </c>
+      <c r="C37" s="1">
+        <f t="shared" si="15"/>
+        <v>0</v>
+      </c>
+      <c r="D37" s="1">
+        <f t="shared" si="15"/>
+        <v>0</v>
+      </c>
+      <c r="E37" s="1">
+        <f t="shared" si="15"/>
+        <v>0</v>
+      </c>
+      <c r="F37" s="1">
+        <f t="shared" si="14"/>
+        <v>0</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Semi-Auto gun visual application
</commit_message>
<xml_diff>
--- a/Docs/timesheet.xlsx
+++ b/Docs/timesheet.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Libraries\Documents\School\Y2\Personal Portfolio\pp2\UnrealEngineBasics\Docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CDF2A62C-AA26-4D71-AE4C-BF17EC6B470E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{33F25754-7510-41AA-94B1-803111E6AFA4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -404,8 +404,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:L37"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="B33" sqref="B33"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E34" sqref="E34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -485,20 +485,20 @@
         <v>3.5166666666666671</v>
       </c>
       <c r="C3" s="1">
-        <f>SUM(C5:C32)</f>
-        <v>18.899999999999995</v>
+        <f>SUM(C5:C100)</f>
+        <v>19.383333333333329</v>
       </c>
       <c r="D3" s="1">
-        <f>SUM(D5:D32)</f>
+        <f>SUM(D5:D100)</f>
         <v>9.7666666666666675</v>
       </c>
       <c r="E3" s="1">
-        <f>SUM(E5:E32)</f>
-        <v>12.416666666666668</v>
+        <f>SUM(E5:E100)</f>
+        <v>13.483333333333334</v>
       </c>
       <c r="F3" s="1">
         <f>SUM(B3:E3)</f>
-        <v>44.599999999999994</v>
+        <v>46.15</v>
       </c>
       <c r="G3" s="1">
         <f>(1/60)*(180+20+10+6)</f>
@@ -506,7 +506,7 @@
       </c>
       <c r="H3" s="1">
         <f>F3+G3</f>
-        <v>48.199999999999996</v>
+        <v>49.75</v>
       </c>
       <c r="I3" s="1"/>
       <c r="J3" s="1"/>
@@ -523,7 +523,7 @@
       </c>
       <c r="C4" s="2">
         <f t="shared" ref="C4:E4" si="1">(C3/C2)</f>
-        <v>0.62999999999999978</v>
+        <v>0.64611111111111097</v>
       </c>
       <c r="D4" s="2">
         <f t="shared" si="1"/>
@@ -531,16 +531,16 @@
       </c>
       <c r="E4" s="2">
         <f t="shared" si="1"/>
-        <v>0.41388888888888892</v>
+        <v>0.44944444444444448</v>
       </c>
       <c r="F4" s="2">
         <f>(F3/F2)</f>
-        <v>0.55749999999999988</v>
+        <v>0.57687500000000003</v>
       </c>
       <c r="G4" s="1"/>
       <c r="H4" s="2">
         <f>(H3/F2)</f>
-        <v>0.60249999999999992</v>
+        <v>0.62187499999999996</v>
       </c>
       <c r="I4" s="1"/>
       <c r="J4" s="1"/>
@@ -1427,12 +1427,12 @@
         <v>0</v>
       </c>
       <c r="E33" s="1">
-        <f>(1/60)*(0)</f>
-        <v>0</v>
+        <f>(1/60)*(9+13+21+21)</f>
+        <v>1.0666666666666667</v>
       </c>
       <c r="F33" s="1">
         <f t="shared" ref="F33" si="13">SUM(B33:E33)</f>
-        <v>0.7</v>
+        <v>1.7666666666666666</v>
       </c>
       <c r="G33" s="1"/>
       <c r="H33" s="1"/>

</xml_diff>

<commit_message>
fixing gun visual application
</commit_message>
<xml_diff>
--- a/Docs/timesheet.xlsx
+++ b/Docs/timesheet.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Libraries\Documents\School\Y2\Personal Portfolio\pp2\UnrealEngineBasics\Docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{33F25754-7510-41AA-94B1-803111E6AFA4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5B4D5985-37BB-4672-882F-0856CDD4888F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -405,7 +405,7 @@
   <dimension ref="A1:L37"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E34" sqref="E34"/>
+      <selection activeCell="H33" sqref="H33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -494,11 +494,11 @@
       </c>
       <c r="E3" s="1">
         <f>SUM(E5:E100)</f>
-        <v>13.483333333333334</v>
+        <v>14.183333333333334</v>
       </c>
       <c r="F3" s="1">
         <f>SUM(B3:E3)</f>
-        <v>46.15</v>
+        <v>46.849999999999994</v>
       </c>
       <c r="G3" s="1">
         <f>(1/60)*(180+20+10+6)</f>
@@ -506,7 +506,7 @@
       </c>
       <c r="H3" s="1">
         <f>F3+G3</f>
-        <v>49.75</v>
+        <v>50.449999999999996</v>
       </c>
       <c r="I3" s="1"/>
       <c r="J3" s="1"/>
@@ -531,16 +531,16 @@
       </c>
       <c r="E4" s="2">
         <f t="shared" si="1"/>
-        <v>0.44944444444444448</v>
+        <v>0.4727777777777778</v>
       </c>
       <c r="F4" s="2">
         <f>(F3/F2)</f>
-        <v>0.57687500000000003</v>
+        <v>0.58562499999999995</v>
       </c>
       <c r="G4" s="1"/>
       <c r="H4" s="2">
         <f>(H3/F2)</f>
-        <v>0.62187499999999996</v>
+        <v>0.63062499999999999</v>
       </c>
       <c r="I4" s="1"/>
       <c r="J4" s="1"/>
@@ -1427,12 +1427,12 @@
         <v>0</v>
       </c>
       <c r="E33" s="1">
-        <f>(1/60)*(9+13+21+21)</f>
-        <v>1.0666666666666667</v>
+        <f>(1/60)*(9+13+21+21+21+21)</f>
+        <v>1.7666666666666666</v>
       </c>
       <c r="F33" s="1">
         <f t="shared" ref="F33" si="13">SUM(B33:E33)</f>
-        <v>1.7666666666666666</v>
+        <v>2.4666666666666668</v>
       </c>
       <c r="G33" s="1"/>
       <c r="H33" s="1"/>

</xml_diff>

<commit_message>
weapon model + skin applied properly
</commit_message>
<xml_diff>
--- a/Docs/timesheet.xlsx
+++ b/Docs/timesheet.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Libraries\Documents\School\Y2\Personal Portfolio\pp2\UnrealEngineBasics\Docs\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Alex\Documents\School\Y2\Personal Portfolio\pp2\UnrealEngineBasics\Docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A048823F-650E-422C-A1A7-8A1E3A470128}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B3B873D8-50A6-46F8-9CCD-5F57B962E823}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-28920" yWindow="-105" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="15">
   <si>
     <t>Date/LO</t>
   </si>
@@ -78,6 +78,9 @@
   </si>
   <si>
     <t>REMAINING DAYS ASSUMED</t>
+  </si>
+  <si>
+    <t>BASED ON LAST DAY</t>
   </si>
 </sst>
 </file>
@@ -414,7 +417,7 @@
   <dimension ref="A1:L37"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I8" sqref="I8"/>
+      <selection activeCell="D34" sqref="D34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -498,19 +501,19 @@
       </c>
       <c r="C3" s="1">
         <f>SUM(C5:C100)</f>
-        <v>19.383333333333329</v>
+        <v>19.549999999999994</v>
       </c>
       <c r="D3" s="1">
         <f>SUM(D5:D100)</f>
-        <v>9.7666666666666675</v>
+        <v>9.8666666666666671</v>
       </c>
       <c r="E3" s="1">
         <f>SUM(E5:E100)</f>
-        <v>14.183333333333334</v>
+        <v>14.366666666666667</v>
       </c>
       <c r="F3" s="1">
         <f>SUM(B3:E3)</f>
-        <v>46.849999999999994</v>
+        <v>47.29999999999999</v>
       </c>
       <c r="G3" s="1">
         <f>(1/60)*(180+20+10+6)</f>
@@ -518,11 +521,11 @@
       </c>
       <c r="H3" s="1">
         <f>F3+G3</f>
-        <v>50.449999999999996</v>
+        <v>50.899999999999991</v>
       </c>
       <c r="I3" s="1">
         <f>80-H3</f>
-        <v>29.550000000000004</v>
+        <v>29.100000000000009</v>
       </c>
       <c r="J3" s="1"/>
       <c r="K3" s="1"/>
@@ -538,24 +541,24 @@
       </c>
       <c r="C4" s="2">
         <f t="shared" ref="C4:E4" si="1">(C3/C2)</f>
-        <v>0.64611111111111097</v>
+        <v>0.65166666666666651</v>
       </c>
       <c r="D4" s="2">
         <f t="shared" si="1"/>
-        <v>0.97666666666666679</v>
+        <v>0.98666666666666669</v>
       </c>
       <c r="E4" s="2">
         <f t="shared" si="1"/>
-        <v>0.4727777777777778</v>
+        <v>0.47888888888888892</v>
       </c>
       <c r="F4" s="2">
         <f>(F3/F2)</f>
-        <v>0.58562499999999995</v>
+        <v>0.59124999999999983</v>
       </c>
       <c r="G4" s="1"/>
       <c r="H4" s="2">
         <f>(H3/F2)</f>
-        <v>0.63062499999999999</v>
+        <v>0.63624999999999987</v>
       </c>
       <c r="I4" s="3" t="s">
         <v>12</v>
@@ -591,7 +594,7 @@
       <c r="H5" s="1"/>
       <c r="I5" s="1">
         <f>F3/(COUNTA(A5:A100))</f>
-        <v>1.4640624999999998</v>
+        <v>1.4781249999999997</v>
       </c>
       <c r="J5" s="1"/>
       <c r="K5" s="1"/>
@@ -654,7 +657,7 @@
       <c r="H7" s="1"/>
       <c r="I7" s="1">
         <f>I3/I5</f>
-        <v>20.183564567769483</v>
+        <v>19.687103594080348</v>
       </c>
       <c r="J7" s="1"/>
       <c r="K7" s="1"/>
@@ -686,7 +689,9 @@
       </c>
       <c r="G8" s="1"/>
       <c r="H8" s="1"/>
-      <c r="I8" s="1"/>
+      <c r="I8" s="3" t="s">
+        <v>14</v>
+      </c>
       <c r="J8" s="1"/>
       <c r="K8" s="1"/>
       <c r="L8" s="1"/>
@@ -717,7 +722,10 @@
       </c>
       <c r="G9" s="1"/>
       <c r="H9" s="1"/>
-      <c r="I9" s="1"/>
+      <c r="I9" s="1">
+        <f>I3/F33</f>
+        <v>9.9771428571428604</v>
+      </c>
       <c r="J9" s="1"/>
       <c r="K9" s="1"/>
       <c r="L9" s="1"/>
@@ -1444,20 +1452,20 @@
         <v>0.21666666666666667</v>
       </c>
       <c r="C33" s="1">
-        <f>(1/60)*(21+8)</f>
-        <v>0.48333333333333334</v>
+        <f>(1/60)*(21+8+10)</f>
+        <v>0.65</v>
       </c>
       <c r="D33" s="1">
-        <f t="shared" si="3"/>
-        <v>0</v>
+        <f>(1/60)*(6)</f>
+        <v>0.1</v>
       </c>
       <c r="E33" s="1">
-        <f>(1/60)*(9+13+21+21+21+21)</f>
-        <v>1.7666666666666666</v>
+        <f>(1/60)*(9+13+21+21+21+21+11)</f>
+        <v>1.95</v>
       </c>
       <c r="F33" s="1">
         <f t="shared" ref="F33" si="13">SUM(B33:E33)</f>
-        <v>2.4666666666666668</v>
+        <v>2.9166666666666665</v>
       </c>
       <c r="G33" s="1"/>
       <c r="H33" s="1"/>
@@ -1475,7 +1483,7 @@
         <v>0</v>
       </c>
       <c r="C34" s="1">
-        <f t="shared" si="3"/>
+        <f>(1/60)*(0)</f>
         <v>0</v>
       </c>
       <c r="D34" s="1">

</xml_diff>

<commit_message>
retargeted animations + guns can be changed
</commit_message>
<xml_diff>
--- a/Docs/timesheet.xlsx
+++ b/Docs/timesheet.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Alex\Documents\School\Y2\Personal Portfolio\pp2\UnrealEngineBasics\Docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B3B873D8-50A6-46F8-9CCD-5F57B962E823}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C18BECDE-0501-4553-A73E-C36255000668}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-28920" yWindow="-105" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -77,10 +77,10 @@
     <t>AVREAGE HR/DAY</t>
   </si>
   <si>
-    <t>REMAINING DAYS ASSUMED</t>
+    <t>BASED ON LAST DAY</t>
   </si>
   <si>
-    <t>BASED ON LAST DAY</t>
+    <t>REMAINING DAYS ASSUMED (AVERAGE)</t>
   </si>
 </sst>
 </file>
@@ -417,7 +417,7 @@
   <dimension ref="A1:L37"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D34" sqref="D34"/>
+      <selection activeCell="I10" sqref="I10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -505,15 +505,15 @@
       </c>
       <c r="D3" s="1">
         <f>SUM(D5:D100)</f>
-        <v>9.8666666666666671</v>
+        <v>10.383333333333335</v>
       </c>
       <c r="E3" s="1">
         <f>SUM(E5:E100)</f>
-        <v>14.366666666666667</v>
+        <v>14.8</v>
       </c>
       <c r="F3" s="1">
         <f>SUM(B3:E3)</f>
-        <v>47.29999999999999</v>
+        <v>48.25</v>
       </c>
       <c r="G3" s="1">
         <f>(1/60)*(180+20+10+6)</f>
@@ -521,11 +521,11 @@
       </c>
       <c r="H3" s="1">
         <f>F3+G3</f>
-        <v>50.899999999999991</v>
+        <v>51.85</v>
       </c>
       <c r="I3" s="1">
-        <f>80-H3</f>
-        <v>29.100000000000009</v>
+        <f>80-F3</f>
+        <v>31.75</v>
       </c>
       <c r="J3" s="1"/>
       <c r="K3" s="1"/>
@@ -545,20 +545,20 @@
       </c>
       <c r="D4" s="2">
         <f t="shared" si="1"/>
-        <v>0.98666666666666669</v>
+        <v>1.0383333333333336</v>
       </c>
       <c r="E4" s="2">
         <f t="shared" si="1"/>
-        <v>0.47888888888888892</v>
+        <v>0.49333333333333335</v>
       </c>
       <c r="F4" s="2">
         <f>(F3/F2)</f>
-        <v>0.59124999999999983</v>
+        <v>0.60312500000000002</v>
       </c>
       <c r="G4" s="1"/>
       <c r="H4" s="2">
         <f>(H3/F2)</f>
-        <v>0.63624999999999987</v>
+        <v>0.64812500000000006</v>
       </c>
       <c r="I4" s="3" t="s">
         <v>12</v>
@@ -594,7 +594,7 @@
       <c r="H5" s="1"/>
       <c r="I5" s="1">
         <f>F3/(COUNTA(A5:A100))</f>
-        <v>1.4781249999999997</v>
+        <v>1.5078125</v>
       </c>
       <c r="J5" s="1"/>
       <c r="K5" s="1"/>
@@ -625,7 +625,7 @@
       <c r="G6" s="1"/>
       <c r="H6" s="1"/>
       <c r="I6" s="3" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="J6" s="1"/>
       <c r="K6" s="1"/>
@@ -657,7 +657,7 @@
       <c r="H7" s="1"/>
       <c r="I7" s="1">
         <f>I3/I5</f>
-        <v>19.687103594080348</v>
+        <v>21.05699481865285</v>
       </c>
       <c r="J7" s="1"/>
       <c r="K7" s="1"/>
@@ -690,7 +690,7 @@
       <c r="G8" s="1"/>
       <c r="H8" s="1"/>
       <c r="I8" s="3" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="J8" s="1"/>
       <c r="K8" s="1"/>
@@ -724,7 +724,7 @@
       <c r="H9" s="1"/>
       <c r="I9" s="1">
         <f>I3/F33</f>
-        <v>9.9771428571428604</v>
+        <v>8.2112068965517242</v>
       </c>
       <c r="J9" s="1"/>
       <c r="K9" s="1"/>
@@ -1456,16 +1456,16 @@
         <v>0.65</v>
       </c>
       <c r="D33" s="1">
-        <f>(1/60)*(6)</f>
-        <v>0.1</v>
+        <f>(1/60)*(6+26+5)</f>
+        <v>0.6166666666666667</v>
       </c>
       <c r="E33" s="1">
-        <f>(1/60)*(9+13+21+21+21+21+11)</f>
-        <v>1.95</v>
+        <f>(1/60)*(9+13+21+21+21+21+11+26)</f>
+        <v>2.3833333333333333</v>
       </c>
       <c r="F33" s="1">
         <f t="shared" ref="F33" si="13">SUM(B33:E33)</f>
-        <v>2.9166666666666665</v>
+        <v>3.8666666666666667</v>
       </c>
       <c r="G33" s="1"/>
       <c r="H33" s="1"/>

</xml_diff>

<commit_message>
reload + ammo counter
</commit_message>
<xml_diff>
--- a/Docs/timesheet.xlsx
+++ b/Docs/timesheet.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Alex\Documents\School\Y2\Personal Portfolio\pp2\UnrealEngineBasics\Docs\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Libraries\Documents\School\Y2\Personal Portfolio\pp2\UnrealEngineBasics\Docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C18BECDE-0501-4553-A73E-C36255000668}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{26CD587C-BC2C-43EC-87A4-70A73A8D4DBF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-105" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -417,7 +417,7 @@
   <dimension ref="A1:L37"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I10" sqref="I10"/>
+      <selection activeCell="B35" sqref="B35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -501,7 +501,7 @@
       </c>
       <c r="C3" s="1">
         <f>SUM(C5:C100)</f>
-        <v>19.549999999999994</v>
+        <v>19.666666666666661</v>
       </c>
       <c r="D3" s="1">
         <f>SUM(D5:D100)</f>
@@ -509,11 +509,11 @@
       </c>
       <c r="E3" s="1">
         <f>SUM(E5:E100)</f>
-        <v>14.8</v>
+        <v>15.666666666666668</v>
       </c>
       <c r="F3" s="1">
         <f>SUM(B3:E3)</f>
-        <v>48.25</v>
+        <v>49.233333333333334</v>
       </c>
       <c r="G3" s="1">
         <f>(1/60)*(180+20+10+6)</f>
@@ -521,11 +521,11 @@
       </c>
       <c r="H3" s="1">
         <f>F3+G3</f>
-        <v>51.85</v>
+        <v>52.833333333333336</v>
       </c>
       <c r="I3" s="1">
         <f>80-F3</f>
-        <v>31.75</v>
+        <v>30.766666666666666</v>
       </c>
       <c r="J3" s="1"/>
       <c r="K3" s="1"/>
@@ -541,7 +541,7 @@
       </c>
       <c r="C4" s="2">
         <f t="shared" ref="C4:E4" si="1">(C3/C2)</f>
-        <v>0.65166666666666651</v>
+        <v>0.65555555555555534</v>
       </c>
       <c r="D4" s="2">
         <f t="shared" si="1"/>
@@ -549,16 +549,16 @@
       </c>
       <c r="E4" s="2">
         <f t="shared" si="1"/>
-        <v>0.49333333333333335</v>
+        <v>0.52222222222222225</v>
       </c>
       <c r="F4" s="2">
         <f>(F3/F2)</f>
-        <v>0.60312500000000002</v>
+        <v>0.61541666666666672</v>
       </c>
       <c r="G4" s="1"/>
       <c r="H4" s="2">
         <f>(H3/F2)</f>
-        <v>0.64812500000000006</v>
+        <v>0.66041666666666665</v>
       </c>
       <c r="I4" s="3" t="s">
         <v>12</v>
@@ -594,7 +594,7 @@
       <c r="H5" s="1"/>
       <c r="I5" s="1">
         <f>F3/(COUNTA(A5:A100))</f>
-        <v>1.5078125</v>
+        <v>1.5385416666666667</v>
       </c>
       <c r="J5" s="1"/>
       <c r="K5" s="1"/>
@@ -657,7 +657,7 @@
       <c r="H7" s="1"/>
       <c r="I7" s="1">
         <f>I3/I5</f>
-        <v>21.05699481865285</v>
+        <v>19.997291807718348</v>
       </c>
       <c r="J7" s="1"/>
       <c r="K7" s="1"/>
@@ -723,8 +723,8 @@
       <c r="G9" s="1"/>
       <c r="H9" s="1"/>
       <c r="I9" s="1">
-        <f>I3/F33</f>
-        <v>8.2112068965517242</v>
+        <f>I3/F34</f>
+        <v>27.969696969696965</v>
       </c>
       <c r="J9" s="1"/>
       <c r="K9" s="1"/>
@@ -1479,24 +1479,24 @@
         <v>45335</v>
       </c>
       <c r="B34" s="1">
-        <f t="shared" si="3"/>
-        <v>0</v>
+        <f>(1/60)*(7)</f>
+        <v>0.11666666666666667</v>
       </c>
       <c r="C34" s="1">
-        <f>(1/60)*(0)</f>
-        <v>0</v>
+        <f>(1/60)*(7)</f>
+        <v>0.11666666666666667</v>
       </c>
       <c r="D34" s="1">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="E34" s="1">
-        <f t="shared" si="3"/>
-        <v>0</v>
+        <f>(1/60)*(22+22+8)</f>
+        <v>0.8666666666666667</v>
       </c>
       <c r="F34" s="1">
         <f t="shared" ref="F34:F37" si="14">SUM(B34:E34)</f>
-        <v>0</v>
+        <v>1.1000000000000001</v>
       </c>
       <c r="G34" s="1"/>
       <c r="H34" s="1"/>

</xml_diff>

<commit_message>
progress on gun animations
</commit_message>
<xml_diff>
--- a/Docs/timesheet.xlsx
+++ b/Docs/timesheet.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Libraries\Documents\School\Y2\Personal Portfolio\pp2\UnrealEngineBasics\Docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{26CD587C-BC2C-43EC-87A4-70A73A8D4DBF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4916B2B4-24EF-4BC3-A952-CBAC7CB58BD2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -417,7 +417,7 @@
   <dimension ref="A1:L37"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B35" sqref="B35"/>
+      <selection activeCell="D35" sqref="D35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -505,7 +505,7 @@
       </c>
       <c r="D3" s="1">
         <f>SUM(D5:D100)</f>
-        <v>10.383333333333335</v>
+        <v>10.916666666666668</v>
       </c>
       <c r="E3" s="1">
         <f>SUM(E5:E100)</f>
@@ -513,7 +513,7 @@
       </c>
       <c r="F3" s="1">
         <f>SUM(B3:E3)</f>
-        <v>49.233333333333334</v>
+        <v>49.766666666666666</v>
       </c>
       <c r="G3" s="1">
         <f>(1/60)*(180+20+10+6)</f>
@@ -521,11 +521,11 @@
       </c>
       <c r="H3" s="1">
         <f>F3+G3</f>
-        <v>52.833333333333336</v>
+        <v>53.366666666666667</v>
       </c>
       <c r="I3" s="1">
         <f>80-F3</f>
-        <v>30.766666666666666</v>
+        <v>30.233333333333334</v>
       </c>
       <c r="J3" s="1"/>
       <c r="K3" s="1"/>
@@ -545,7 +545,7 @@
       </c>
       <c r="D4" s="2">
         <f t="shared" si="1"/>
-        <v>1.0383333333333336</v>
+        <v>1.0916666666666668</v>
       </c>
       <c r="E4" s="2">
         <f t="shared" si="1"/>
@@ -553,12 +553,12 @@
       </c>
       <c r="F4" s="2">
         <f>(F3/F2)</f>
-        <v>0.61541666666666672</v>
+        <v>0.62208333333333332</v>
       </c>
       <c r="G4" s="1"/>
       <c r="H4" s="2">
         <f>(H3/F2)</f>
-        <v>0.66041666666666665</v>
+        <v>0.66708333333333336</v>
       </c>
       <c r="I4" s="3" t="s">
         <v>12</v>
@@ -594,7 +594,7 @@
       <c r="H5" s="1"/>
       <c r="I5" s="1">
         <f>F3/(COUNTA(A5:A100))</f>
-        <v>1.5385416666666667</v>
+        <v>1.5552083333333333</v>
       </c>
       <c r="J5" s="1"/>
       <c r="K5" s="1"/>
@@ -657,7 +657,7 @@
       <c r="H7" s="1"/>
       <c r="I7" s="1">
         <f>I3/I5</f>
-        <v>19.997291807718348</v>
+        <v>19.440053583389151</v>
       </c>
       <c r="J7" s="1"/>
       <c r="K7" s="1"/>
@@ -724,7 +724,7 @@
       <c r="H9" s="1"/>
       <c r="I9" s="1">
         <f>I3/F34</f>
-        <v>27.969696969696965</v>
+        <v>18.510204081632654</v>
       </c>
       <c r="J9" s="1"/>
       <c r="K9" s="1"/>
@@ -836,7 +836,7 @@
         <v>2.35</v>
       </c>
       <c r="D13" s="1">
-        <f t="shared" ref="B13:E34" si="3">(1/60)*(0)</f>
+        <f t="shared" ref="B13:E32" si="3">(1/60)*(0)</f>
         <v>0</v>
       </c>
       <c r="E13" s="1">
@@ -1487,8 +1487,8 @@
         <v>0.11666666666666667</v>
       </c>
       <c r="D34" s="1">
-        <f t="shared" si="3"/>
-        <v>0</v>
+        <f>(1/60)*(22+10)</f>
+        <v>0.53333333333333333</v>
       </c>
       <c r="E34" s="1">
         <f>(1/60)*(22+22+8)</f>
@@ -1496,7 +1496,7 @@
       </c>
       <c r="F34" s="1">
         <f t="shared" ref="F34:F37" si="14">SUM(B34:E34)</f>
-        <v>1.1000000000000001</v>
+        <v>1.6333333333333333</v>
       </c>
       <c r="G34" s="1"/>
       <c r="H34" s="1"/>

</xml_diff>

<commit_message>
crouching and aim offset
</commit_message>
<xml_diff>
--- a/Docs/timesheet.xlsx
+++ b/Docs/timesheet.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Libraries\Documents\School\Y2\Personal Portfolio\pp2\UnrealEngineBasics\Docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4916B2B4-24EF-4BC3-A952-CBAC7CB58BD2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{174F99F8-96D5-43E8-B18D-CE9CFC11466E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="16">
   <si>
     <t>Date/LO</t>
   </si>
@@ -81,6 +81,9 @@
   </si>
   <si>
     <t>REMAINING DAYS ASSUMED (AVERAGE)</t>
+  </si>
+  <si>
+    <t>BASED ON TODAY</t>
   </si>
 </sst>
 </file>
@@ -501,11 +504,11 @@
       </c>
       <c r="C3" s="1">
         <f>SUM(C5:C100)</f>
-        <v>19.666666666666661</v>
+        <v>19.999999999999993</v>
       </c>
       <c r="D3" s="1">
         <f>SUM(D5:D100)</f>
-        <v>10.916666666666668</v>
+        <v>13.083333333333336</v>
       </c>
       <c r="E3" s="1">
         <f>SUM(E5:E100)</f>
@@ -513,7 +516,7 @@
       </c>
       <c r="F3" s="1">
         <f>SUM(B3:E3)</f>
-        <v>49.766666666666666</v>
+        <v>52.266666666666666</v>
       </c>
       <c r="G3" s="1">
         <f>(1/60)*(180+20+10+6)</f>
@@ -521,11 +524,11 @@
       </c>
       <c r="H3" s="1">
         <f>F3+G3</f>
-        <v>53.366666666666667</v>
+        <v>55.866666666666667</v>
       </c>
       <c r="I3" s="1">
         <f>80-F3</f>
-        <v>30.233333333333334</v>
+        <v>27.733333333333334</v>
       </c>
       <c r="J3" s="1"/>
       <c r="K3" s="1"/>
@@ -541,11 +544,11 @@
       </c>
       <c r="C4" s="2">
         <f t="shared" ref="C4:E4" si="1">(C3/C2)</f>
-        <v>0.65555555555555534</v>
+        <v>0.66666666666666641</v>
       </c>
       <c r="D4" s="2">
         <f t="shared" si="1"/>
-        <v>1.0916666666666668</v>
+        <v>1.3083333333333336</v>
       </c>
       <c r="E4" s="2">
         <f t="shared" si="1"/>
@@ -553,12 +556,12 @@
       </c>
       <c r="F4" s="2">
         <f>(F3/F2)</f>
-        <v>0.62208333333333332</v>
+        <v>0.65333333333333332</v>
       </c>
       <c r="G4" s="1"/>
       <c r="H4" s="2">
         <f>(H3/F2)</f>
-        <v>0.66708333333333336</v>
+        <v>0.69833333333333336</v>
       </c>
       <c r="I4" s="3" t="s">
         <v>12</v>
@@ -594,7 +597,7 @@
       <c r="H5" s="1"/>
       <c r="I5" s="1">
         <f>F3/(COUNTA(A5:A100))</f>
-        <v>1.5552083333333333</v>
+        <v>1.6333333333333333</v>
       </c>
       <c r="J5" s="1"/>
       <c r="K5" s="1"/>
@@ -656,8 +659,8 @@
       <c r="G7" s="1"/>
       <c r="H7" s="1"/>
       <c r="I7" s="1">
-        <f>I3/I5</f>
-        <v>19.440053583389151</v>
+        <f>ROUNDUP(I3/I5, 0)</f>
+        <v>17</v>
       </c>
       <c r="J7" s="1"/>
       <c r="K7" s="1"/>
@@ -690,7 +693,7 @@
       <c r="G8" s="1"/>
       <c r="H8" s="1"/>
       <c r="I8" s="3" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="J8" s="1"/>
       <c r="K8" s="1"/>
@@ -723,8 +726,8 @@
       <c r="G9" s="1"/>
       <c r="H9" s="1"/>
       <c r="I9" s="1">
-        <f>I3/F34</f>
-        <v>18.510204081632654</v>
+        <f>ROUNDUP(I3/F34, 0)</f>
+        <v>7</v>
       </c>
       <c r="J9" s="1"/>
       <c r="K9" s="1"/>
@@ -756,7 +759,9 @@
       </c>
       <c r="G10" s="1"/>
       <c r="H10" s="1"/>
-      <c r="I10" s="1"/>
+      <c r="I10" s="3" t="s">
+        <v>13</v>
+      </c>
       <c r="J10" s="1"/>
       <c r="K10" s="1"/>
       <c r="L10" s="1"/>
@@ -787,7 +792,10 @@
       </c>
       <c r="G11" s="1"/>
       <c r="H11" s="1"/>
-      <c r="I11" s="1"/>
+      <c r="I11" s="1">
+        <f>ROUNDUP(I3/F33, 0)</f>
+        <v>8</v>
+      </c>
       <c r="J11" s="1"/>
       <c r="K11" s="1"/>
       <c r="L11" s="1"/>
@@ -1483,12 +1491,12 @@
         <v>0.11666666666666667</v>
       </c>
       <c r="C34" s="1">
-        <f>(1/60)*(7)</f>
-        <v>0.11666666666666667</v>
+        <f>(1/60)*(7+20)</f>
+        <v>0.45</v>
       </c>
       <c r="D34" s="1">
-        <f>(1/60)*(22+10)</f>
-        <v>0.53333333333333333</v>
+        <f>(1/60)*(22+10+20+20+20+20+5+20+5+20)</f>
+        <v>2.7</v>
       </c>
       <c r="E34" s="1">
         <f>(1/60)*(22+22+8)</f>
@@ -1496,7 +1504,7 @@
       </c>
       <c r="F34" s="1">
         <f t="shared" ref="F34:F37" si="14">SUM(B34:E34)</f>
-        <v>1.6333333333333333</v>
+        <v>4.1333333333333329</v>
       </c>
       <c r="G34" s="1"/>
       <c r="H34" s="1"/>

</xml_diff>